<commit_message>
Included object details for Usersite Menu - Document Register
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>textbox</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>idHomePageNewItem</t>
+  </si>
+  <si>
+    <t>Document Register</t>
+  </si>
+  <si>
+    <t>Usersite Menu - Document Register</t>
   </si>
 </sst>
 </file>
@@ -824,7 +830,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -924,6 +930,20 @@
       </c>
       <c r="E6" s="4" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1104,7 +1124,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D15 D3:D9 D17</xm:sqref>
+          <xm:sqref>D11:D15 D17 D3:D9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Included Fluid Menu List
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>textbox</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>element_notdisplayed</t>
+  </si>
+  <si>
+    <t>User Site Fluid/Fulcrum Menu Navigation</t>
+  </si>
+  <si>
+    <t>Fluid Menu List</t>
+  </si>
+  <si>
+    <t>.//span[contains(@class,'-item')]</t>
   </si>
 </sst>
 </file>
@@ -880,10 +889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1148,8 +1157,34 @@
         <v>41</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A16:G16"/>

</xml_diff>

<commit_message>
New keys are included.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1176,7 +1176,7 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
         <v>76</v>
@@ -1206,13 +1206,13 @@
           <x14:formula1>
             <xm:f>Objects:Objects_Navigation!$A$2:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>D20 D23 D18</xm:sqref>
+          <xm:sqref>D18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$28</xm:f>
+            <xm:f>Objects!$A$2:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D15 D17 D3:D9</xm:sqref>
+          <xm:sqref>D11:D15 D17 D3:D9 D20 D23 D26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated Fluid Menu List
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1201,18 +1201,12 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects:Objects_Navigation!$A$2:$A$40</xm:f>
-          </x14:formula1>
-          <xm:sqref>D18</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D15 D17 D3:D9 D20 D23 D26</xm:sqref>
+          <xm:sqref>D11:D15 D17:D18 D3:D9 D20:D21 D23:D24 D26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added Usersite Menu - Documents
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>textbox</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>.//span[contains(@class,'-item')]</t>
+  </si>
+  <si>
+    <t>Usersite Menu - Documents</t>
+  </si>
+  <si>
+    <t>Documents</t>
   </si>
 </sst>
 </file>
@@ -891,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1006,6 +1012,20 @@
       </c>
       <c r="E7" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>